<commit_message>
Proyecto integrado de las mejoras realizadas a reprogramacion
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoConsumo.xlsx
+++ b/target/DatosExcel/DatosCreditoConsumo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGELA\OneDrive\Público\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t xml:space="preserve"> Monto</t>
   </si>
@@ -128,17 +128,56 @@
     <t>prueba justificacion 2</t>
   </si>
   <si>
-    <t>Aprobar propuesta</t>
-  </si>
-  <si>
     <t>prueba</t>
+  </si>
+  <si>
+    <t>Promoción</t>
+  </si>
+  <si>
+    <t>SIN PROMOCION</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>23622173</t>
+  </si>
+  <si>
+    <t>25461886</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Aprobar propuesta1</t>
+  </si>
+  <si>
+    <t>Aprobar propuesta2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,13 +192,27 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -174,11 +227,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,216 +515,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2">
-        <v>24488748</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:21" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2">
-        <v>1000</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="L2">
-        <v>12</v>
-      </c>
-      <c r="M2" s="1">
+      <c r="L2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="S2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="Q3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3">
-        <v>10499976</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3">
-        <v>4500</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3">
-        <v>16</v>
-      </c>
-      <c r="L3">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se sube los cambios realizados en la regresión de la automatización y también el avance en el feature y definitions de Reprogramación Otro Pagaré
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoConsumo.xlsx
+++ b/target/DatosExcel/DatosCreditoConsumo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGELA\OneDrive\Público\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOSITORIO_ACTUAL\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t xml:space="preserve"> Monto</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Día Pago</t>
   </si>
   <si>
-    <t># Cuotas</t>
-  </si>
-  <si>
     <t>Tasa Preferencial</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>1000</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -171,6 +165,27 @@
   </si>
   <si>
     <t>Aprobar propuesta2</t>
+  </si>
+  <si>
+    <t>Número Cuotas</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Numero Propuesta</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>4899799</t>
+  </si>
+  <si>
+    <t>El Documento ha sido derivado satisfactoriamente</t>
+  </si>
+  <si>
+    <t>4899800</t>
   </si>
 </sst>
 </file>
@@ -201,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +226,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,14 +254,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,226 +544,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="46.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:23" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="3" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="G2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="4" t="s">
+      <c r="R2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="3" customFormat="1">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1">
-      <c r="A2" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="1" customFormat="1">
-      <c r="A3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="Q3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>34</v>
+      <c r="V3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avance con mejoras en el login y emision de dictamen
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoConsumo.xlsx
+++ b/target/DatosExcel/DatosCreditoConsumo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOSITORIO_ACTUAL\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t xml:space="preserve"> Monto</t>
   </si>
@@ -134,9 +134,6 @@
     <t>SIN PROMOCION</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -152,15 +149,6 @@
     <t>30</t>
   </si>
   <si>
-    <t>23622173</t>
-  </si>
-  <si>
-    <t>25461886</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>Aprobar propuesta1</t>
   </si>
   <si>
@@ -179,19 +167,29 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t>4899799</t>
-  </si>
-  <si>
-    <t>El Documento ha sido derivado satisfactoriamente</t>
-  </si>
-  <si>
-    <t>4899800</t>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>23162539</t>
+  </si>
+  <si>
+    <t>12668309</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>4900002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -546,32 +544,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="46.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1">
@@ -612,7 +608,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -639,15 +635,15 @@
         <v>16</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
@@ -665,10 +661,10 @@
         <v>35</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>21</v>
@@ -680,13 +676,13 @@
         <v>23</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>24</v>
@@ -704,21 +700,21 @@
         <v>31</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="V2" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" t="s">
         <v>51</v>
-      </c>
-      <c r="W2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>18</v>
@@ -736,10 +732,10 @@
         <v>35</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>21</v>
@@ -751,13 +747,13 @@
         <v>23</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>24</v>
@@ -775,17 +771,13 @@
         <v>32</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="U3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="V3" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3" t="s">
-        <v>52</v>
-      </c>
+      <c r="V3"/>
+      <c r="W3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualización de flujos automatizados
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoConsumo.xlsx
+++ b/target/DatosExcel/DatosCreditoConsumo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMACPiura_2022\CMACPiura_2022\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,26 +24,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo Servicio        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Servicio Credito </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tipo Propuesta </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SubTipo Propuesta</t>
+  </si>
+  <si>
+    <t>Promoción</t>
+  </si>
   <si>
     <t xml:space="preserve"> Monto</t>
   </si>
   <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo Servicio        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Servicio Credito </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tipo Propuesta </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SubTipo Propuesta</t>
-  </si>
-  <si>
     <t>Tasa Inicial</t>
   </si>
   <si>
@@ -59,12 +62,18 @@
     <t>Día Pago</t>
   </si>
   <si>
+    <t>Número Cuotas</t>
+  </si>
+  <si>
     <t>Tasa Preferencial</t>
   </si>
   <si>
     <t>Forma Desembolso</t>
   </si>
   <si>
+    <t>Nota de operación</t>
+  </si>
+  <si>
     <t>Clasificacion Crediticia</t>
   </si>
   <si>
@@ -74,10 +83,19 @@
     <t>Justificacion Credito</t>
   </si>
   <si>
+    <t>Observaciones aprobación</t>
+  </si>
+  <si>
     <t>Contraseña</t>
   </si>
   <si>
-    <t>Observaciones aprobación</t>
+    <t>Numero Propuesta</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>23934914</t>
   </si>
   <si>
     <t>CREDITOS DE CONSUMO</t>
@@ -89,6 +107,15 @@
     <t>NORMAL</t>
   </si>
   <si>
+    <t>SIN PROMOCION</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>Fija Vencida</t>
   </si>
   <si>
@@ -98,109 +125,56 @@
     <t>Fecha Fija</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>ABONO EN CUENTA</t>
   </si>
   <si>
     <t>prueba de nueva propuesta</t>
   </si>
   <si>
-    <t>Nota de operación</t>
-  </si>
-  <si>
     <t>prueba clasificacion 1</t>
   </si>
   <si>
-    <t>prueba clasificacion 2</t>
-  </si>
-  <si>
     <t>prueba objetivo 1</t>
   </si>
   <si>
-    <t>prueba objetivo 2</t>
-  </si>
-  <si>
     <t>prueba justificacion 1</t>
   </si>
   <si>
-    <t>prueba justificacion 2</t>
+    <t>Aprobar propuesta1</t>
   </si>
   <si>
     <t>prueba</t>
   </si>
   <si>
-    <t>Promoción</t>
-  </si>
-  <si>
-    <t>SIN PROMOCION</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>Aprobar propuesta1</t>
-  </si>
-  <si>
-    <t>Aprobar propuesta2</t>
-  </si>
-  <si>
-    <t>Número Cuotas</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Numero Propuesta</t>
-  </si>
-  <si>
-    <t>Resultado</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>23934914</t>
-  </si>
-  <si>
-    <t>23977184</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>4000</t>
-  </si>
-  <si>
-    <t>10.5</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>4978772</t>
-  </si>
-  <si>
-    <t>Se han encontrado errores en la Validacion de la Propuesta</t>
-  </si>
-  <si>
-    <t>4978773</t>
+    <t>4978790</t>
+  </si>
+  <si>
+    <t>El Documento ha sido derivado satisfactoriamente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -213,14 +187,6 @@
       <color rgb="FF297BDE"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -263,14 +229,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,249 +517,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:23" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="5" customFormat="1">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="N2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="6" t="s">
+      <c r="U2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" s="3" customFormat="1">
-      <c r="A2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" s="3" customFormat="1">
-      <c r="A3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="V3" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>